<commit_message>
cambio3 : cambio de color
</commit_message>
<xml_diff>
--- a/PRACTICA EXCEL.xlsx
+++ b/PRACTICA EXCEL.xlsx
@@ -169,7 +169,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,6 +182,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="37">
     <border>
@@ -690,7 +696,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -750,6 +756,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1041,11 +1048,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="4079472"/>
-        <c:axId val="151299464"/>
+        <c:axId val="4407152"/>
+        <c:axId val="199618096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="4079472"/>
+        <c:axId val="4407152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1087,7 +1094,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="151299464"/>
+        <c:crossAx val="199618096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1095,7 +1102,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="151299464"/>
+        <c:axId val="199618096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-500"/>
@@ -1146,7 +1153,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4079472"/>
+        <c:crossAx val="4407152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3031,7 +3038,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3060,7 +3067,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="59" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="49">
@@ -3082,7 +3089,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="59" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="49">

</xml_diff>